<commit_message>
Updates. Using random forest gives good results.
</commit_message>
<xml_diff>
--- a/Code/R/Magnan/Data.xlsx
+++ b/Code/R/Magnan/Data.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="CmpStateOfArt" sheetId="1" r:id="rId1"/>
+    <sheet name="TenfoldAvgCmp" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,78 +16,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Model File</t>
   </si>
   <si>
-    <t>TFCV_Sn</t>
-  </si>
-  <si>
-    <t>TFCV_Sp</t>
-  </si>
-  <si>
-    <t>TFCV_Mcc</t>
-  </si>
-  <si>
-    <t>TF_Acc</t>
-  </si>
-  <si>
-    <t>IT_Sn</t>
-  </si>
-  <si>
-    <t>IT_Acc</t>
-  </si>
-  <si>
-    <t>IT_Sp</t>
-  </si>
-  <si>
-    <t>IT_Mcc</t>
-  </si>
-  <si>
     <t>Features</t>
   </si>
   <si>
-    <t>SearchType</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Learning Type</t>
   </si>
   <si>
-    <t>SVM Regress.</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>VaxiJen</t>
   </si>
   <si>
     <t>ANTIGENPro</t>
   </si>
   <si>
-    <t>TF_AUROC</t>
-  </si>
-  <si>
-    <t>PerfSearch_Regression_nGrams</t>
-  </si>
-  <si>
-    <t>PerfSearch_Regression_PSF10</t>
-  </si>
-  <si>
-    <t>PerfSearch_Regression_nGDip25</t>
-  </si>
-  <si>
-    <t>6250-5250/25</t>
-  </si>
-  <si>
-    <t>1250-250/25</t>
-  </si>
-  <si>
-    <t>3500-2500/25</t>
+    <t>PerfSearch_RF_Balanced_SvmRFE2_heu_comb</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>TrainingSet</t>
+  </si>
+  <si>
+    <t>Balanced</t>
+  </si>
+  <si>
+    <t>Unbalanced</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>MCC Optimized</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>AUCROC</t>
+  </si>
+  <si>
+    <t>AUCPR</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>MCC</t>
   </si>
 </sst>
 </file>
@@ -131,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -141,6 +132,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,233 +429,229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K2" sqref="K2:N2"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H2" sqref="H2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="67.28515625" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="10" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1">
+    <row r="1" spans="1:17" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="17.25" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="6">
+        <v>340</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.86113431954089503</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0.849317829496817</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0.78350694444444502</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0.80659722222222197</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0.76041666666666696</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0.77107278128323598</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0.78839090179059002</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0.56768767993741198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="H8">
+        <v>59.48</v>
+      </c>
+      <c r="I8" s="4">
+        <v>89.69</v>
+      </c>
+      <c r="J8" s="4">
+        <v>25.85</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="17.25" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2">
-        <v>5575</v>
-      </c>
-      <c r="E2">
-        <v>30</v>
-      </c>
-      <c r="F2">
-        <v>0.71788194444444398</v>
-      </c>
-      <c r="G2">
-        <v>0.72395833333333304</v>
-      </c>
-      <c r="H2">
-        <v>0.71180555555555602</v>
-      </c>
-      <c r="I2">
-        <v>0.43579607143977001</v>
-      </c>
-      <c r="J2">
-        <v>0.765200014467594</v>
-      </c>
-      <c r="K2">
-        <v>0.602870813397129</v>
-      </c>
-      <c r="L2">
-        <v>0.58904109589041098</v>
-      </c>
-      <c r="M2">
-        <v>0.60359712230215801</v>
-      </c>
-      <c r="N2">
-        <v>8.5409891873273497E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3">
-        <v>800</v>
-      </c>
-      <c r="E3">
-        <v>0.3</v>
-      </c>
-      <c r="F3">
-        <v>0.75607638888888895</v>
-      </c>
-      <c r="G3">
-        <v>0.78993055555555602</v>
-      </c>
-      <c r="H3">
-        <v>0.72222222222222199</v>
-      </c>
-      <c r="I3">
-        <v>0.51333079101764201</v>
-      </c>
-      <c r="J3">
-        <v>0.82624722704475595</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4">
-        <v>3275</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0.6875</v>
-      </c>
-      <c r="G4">
-        <v>0.65972222222222199</v>
-      </c>
-      <c r="H4">
-        <v>0.71527777777777801</v>
-      </c>
-      <c r="I4">
-        <v>0.37558004675039403</v>
-      </c>
-      <c r="J4">
-        <v>0.72302396797839397</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="3"/>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="3"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7">
-        <v>59.48</v>
-      </c>
-      <c r="G7" s="4">
-        <v>89.69</v>
-      </c>
-      <c r="H7" s="4">
-        <v>25.85</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0.67</v>
-      </c>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8">
+      <c r="F9">
+        <v>0.81</v>
+      </c>
+      <c r="H9">
         <v>75.510000000000005</v>
       </c>
-      <c r="G8">
+      <c r="I9">
         <v>75.88</v>
       </c>
-      <c r="H8">
+      <c r="J9">
         <v>75.14</v>
       </c>
-      <c r="I8">
+      <c r="M9">
         <v>0.51</v>
       </c>
-      <c r="J8">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:14">
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>